<commit_message>
lógica para não gerar a mesma rota 2 vezes
</commit_message>
<xml_diff>
--- a/Data/roteiro_entregas_caminhão1.xlsx
+++ b/Data/roteiro_entregas_caminhão1.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,12 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>11103</t>
+          <t>11069</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -496,19 +496,19 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Caminho Novo</t>
+          <t>Barreiros</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>11102</t>
+          <t>11068</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -523,19 +523,19 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Cachoeiras (Guaporanga)</t>
+          <t>Barreiros</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>11056</t>
+          <t>11074</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>12/11/2024</t>
+          <t>13/11/2024</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -550,14 +550,14 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Areias de Cima (Guaporanga)</t>
+          <t>Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>11080</t>
+          <t>11107</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -577,14 +577,14 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>11077</t>
+          <t>11084</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>manhã</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -604,14 +604,14 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Brejarú</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>11076</t>
+          <t>11083</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>manhã</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -631,14 +631,14 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Brejarú</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>11111</t>
+          <t>11076</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -658,14 +658,14 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>11115</t>
+          <t>11061</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -685,14 +685,14 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Aririú</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>11110</t>
+          <t>11078</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -712,14 +712,14 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>11069</t>
+          <t>11080</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -739,14 +739,14 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Barreiros</t>
+          <t>Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>11068</t>
+          <t>11077</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -766,14 +766,14 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Barreiros</t>
+          <t>Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>11084</t>
+          <t>11057</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>tarde</t>
+          <t>manhã</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -793,14 +793,14 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Brejarú</t>
+          <t>Aririú</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>11083</t>
+          <t>11114</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -820,7 +820,169 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Brejarú</t>
+          <t>Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>11110</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>14/11/2024</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>14/11/2024</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>11115</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>14/11/2024</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>11050</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>15/11/2024</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>manhã</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>Areias de Cima (Guaporanga)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>11088</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>15/11/2024</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>manhã</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>Cachoeiras (Guaporanga)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>11105</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>15/11/2024</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>Campeche</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Essa mudança é provisória
</commit_message>
<xml_diff>
--- a/Data/roteiro_entregas_caminhão1.xlsx
+++ b/Data/roteiro_entregas_caminhão1.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="29" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,12 +476,12 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>11069</t>
+          <t>11149</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -496,19 +496,19 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Barreiros</t>
+          <t>Distrito Industrial</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>11068</t>
+          <t>11201</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -523,19 +523,19 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Barreiros</t>
+          <t>Ponte do Imaruim</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>11074</t>
+          <t>11142</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -550,19 +550,19 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Centro</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>11107</t>
+          <t>11179</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -577,24 +577,24 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Nova Palhoça</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>11084</t>
+          <t>11064</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>tarde</t>
+          <t>manhã</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -604,19 +604,19 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>Brejarú</t>
+          <t>Barra do Aririú</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>11083</t>
+          <t>11158</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -631,19 +631,19 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Brejarú</t>
+          <t>Forquilhinha</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>11076</t>
+          <t>11151</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -658,19 +658,19 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Forquilhas</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>11061</t>
+          <t>11222</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -685,19 +685,19 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Aririú</t>
+          <t>Sertão do Maruim</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>11078</t>
+          <t>11194</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -712,24 +712,24 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Pedra Branca</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>11080</t>
+          <t>11193</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>19/11/2024</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>manhã</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -739,19 +739,19 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Pedra Branca</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>11077</t>
+          <t>11197</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -766,19 +766,19 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>Bela Vista</t>
+          <t>Picadas do Sul</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>11057</t>
+          <t>11140</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -793,24 +793,24 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Aririú</t>
+          <t>Centro</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>11114</t>
+          <t>11071</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>tarde</t>
+          <t>manhã</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -820,24 +820,24 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Barreiros</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>11110</t>
+          <t>11177</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>tarde</t>
+          <t>manhã</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
@@ -847,19 +847,19 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Nossa Senhora do Rosário</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>11111</t>
+          <t>11200</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -874,19 +874,19 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Ponta de Baixo</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>11115</t>
+          <t>11141</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>14/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -901,24 +901,24 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Centro</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>11050</t>
+          <t>11144</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>15/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>manhã</t>
+          <t>tarde</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
@@ -928,61 +928,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>Areias de Cima (Guaporanga)</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>11088</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>15/11/2024</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>manhã</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>Cachoeiras (Guaporanga)</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="inlineStr">
-        <is>
-          <t>11105</t>
-        </is>
-      </c>
-      <c r="B20" s="3" t="inlineStr">
-        <is>
-          <t>15/11/2024</t>
-        </is>
-      </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>tarde</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>Campeche</t>
+          <t>Centro</t>
         </is>
       </c>
     </row>

</xml_diff>